<commit_message>
Added an updated version of the test cases
</commit_message>
<xml_diff>
--- a/TestCases/Back End/CreateAssessment-BackEnd-TeamLead.xlsx
+++ b/TestCases/Back End/CreateAssessment-BackEnd-TeamLead.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18805"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="14" documentId="8_{F51AD809-CB10-49BA-B733-9C20C8B32ABA}" xr6:coauthVersionLast="26" xr6:coauthVersionMax="26" xr10:uidLastSave="{161010DD-4FCC-49E8-99AD-EAC2A49C7CA4}"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="8_{F51AD809-CB10-49BA-B733-9C20C8B32ABA}" xr6:coauthVersionLast="26" xr6:coauthVersionMax="26" xr10:uidLastSave="{DAA4EEF7-5E21-469F-B09A-C453C6AFEFC7}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>Role: Team Lead</t>
   </si>
@@ -51,6 +51,9 @@
   </si>
   <si>
     <t>A new assessment will be added to the database for that employee</t>
+  </si>
+  <si>
+    <t>it threw an exception.</t>
   </si>
   <si>
     <t>Step 4: Fill out a assessment for an employee that is not in your team</t>
@@ -415,8 +418,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="C2" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -473,29 +476,32 @@
       <c r="D4" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="E4" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="5" spans="1:6" ht="58.5" customHeight="1">
       <c r="C5" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="60.75" customHeight="1">
       <c r="C6" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="60.75" customHeight="1">
       <c r="C7" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F7" s="2"/>
     </row>

</xml_diff>